<commit_message>
-Scientific Paper with part of Alex (Recombination / Mutation) -New diagrams of quality of algorithm
</commit_message>
<xml_diff>
--- a/TimeTabling/doc/Solutions_Quality_Diagrams.xlsx
+++ b/TimeTabling/doc/Solutions_Quality_Diagrams.xlsx
@@ -11,6 +11,9 @@
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId4"/>
+  </externalReferences>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
@@ -89,7 +92,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="de-DE"/>
-              <a:t>Instance1</a:t>
+              <a:t>Instance 1,11</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -149,13 +152,61 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:hiLowLines/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Instance11</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>(Tabelle1!$B$1,Tabelle1!$C$1,Tabelle1!$F$1,Tabelle1!$G$1)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Tabelle1!$B$12,Tabelle1!$C$12,Tabelle1!$F$12,Tabelle1!$G$12)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1094</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>309</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>151</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
         <c:marker val="1"/>
-        <c:axId val="56378880"/>
-        <c:axId val="56380800"/>
+        <c:axId val="74339072"/>
+        <c:axId val="74341376"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="56378880"/>
+        <c:axId val="74339072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -181,14 +232,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56380800"/>
+        <c:crossAx val="74341376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="56380800"/>
+        <c:axId val="74341376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -214,7 +265,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56378880"/>
+        <c:crossAx val="74339072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -227,7 +278,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.70000000000000007" r="0.70000000000000007" t="0.78740157499999996" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000018" r="0.70000000000000018" t="0.78740157499999996" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -311,11 +362,11 @@
         </c:ser>
         <c:hiLowLines/>
         <c:marker val="1"/>
-        <c:axId val="50291456"/>
-        <c:axId val="52761728"/>
+        <c:axId val="74362240"/>
+        <c:axId val="72947200"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="50291456"/>
+        <c:axId val="74362240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -341,14 +392,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52761728"/>
+        <c:crossAx val="72947200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="52761728"/>
+        <c:axId val="72947200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -374,7 +425,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50291456"/>
+        <c:crossAx val="74362240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -387,7 +438,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.70000000000000029" r="0.70000000000000029" t="0.78740157499999996" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.78740157499999996" l="0.7000000000000004" r="0.7000000000000004" t="0.78740157499999996" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -428,7 +479,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>[solutions.xlsx]Tabelle1!$B$1:$C$1,[solutions.xlsx]Tabelle1!$F$1:$G$1</c:f>
+              <c:f>(Tabelle1!$B$1,Tabelle1!$C$1,Tabelle1!$F$1,Tabelle1!$G$1)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -471,11 +522,11 @@
         </c:ser>
         <c:hiLowLines/>
         <c:marker val="1"/>
-        <c:axId val="50390528"/>
-        <c:axId val="52737920"/>
+        <c:axId val="73000832"/>
+        <c:axId val="73003008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="50390528"/>
+        <c:axId val="73000832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -501,14 +552,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52737920"/>
+        <c:crossAx val="73003008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="52737920"/>
+        <c:axId val="73003008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -534,7 +585,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50390528"/>
+        <c:crossAx val="73000832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -547,7 +598,167 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.70000000000000051" r="0.70000000000000051" t="0.78740157499999996" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000062" r="0.70000000000000062" t="0.78740157499999996" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="de-DE"/>
+  <c:style val="6"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE"/>
+              <a:t>Instance03</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Instance03</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>(Tabelle1!$B$1,Tabelle1!$C$1,Tabelle1!$F$1,Tabelle1!$G$1)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Tabelle1!$B$4,Tabelle1!$C$4,Tabelle1!$F$4,Tabelle1!$G$4)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>5066</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2648</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>776</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>522</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:hiLowLines/>
+        <c:marker val="1"/>
+        <c:axId val="67409408"/>
+        <c:axId val="67411328"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="67409408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Iterations</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="67411328"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="67411328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Penalty</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="67409408"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000062" r="0.70000000000000062" t="0.78740157499999996" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -587,16 +798,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -645,7 +856,50 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Diagramm 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Tabelle1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -933,10 +1187,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -944,7 +1198,7 @@
     <col min="1" max="1" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1">
+    <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -970,7 +1224,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -996,7 +1250,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1019,10 +1273,16 @@
         <v>614</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:8">
       <c r="A4" s="1">
         <v>3</v>
       </c>
+      <c r="B4">
+        <v>5066</v>
+      </c>
+      <c r="C4">
+        <v>2648</v>
+      </c>
       <c r="D4">
         <v>923</v>
       </c>
@@ -1032,11 +1292,20 @@
       <c r="F4">
         <v>776</v>
       </c>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="G4">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="1">
         <v>4</v>
       </c>
+      <c r="B5">
+        <v>4434</v>
+      </c>
+      <c r="C5">
+        <v>1693</v>
+      </c>
       <c r="D5">
         <v>1436</v>
       </c>
@@ -1047,10 +1316,16 @@
         <v>973</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:8">
       <c r="A6" s="1">
         <v>5</v>
       </c>
+      <c r="B6">
+        <v>8431</v>
+      </c>
+      <c r="C6">
+        <v>2708</v>
+      </c>
       <c r="D6">
         <v>2305</v>
       </c>
@@ -1060,20 +1335,17 @@
       <c r="F6">
         <v>2104</v>
       </c>
-      <c r="I6">
-        <v>1904</v>
-      </c>
-      <c r="J6">
-        <v>1934</v>
-      </c>
-      <c r="K6">
-        <v>1794</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="1">
         <v>6</v>
       </c>
+      <c r="B7">
+        <v>6149</v>
+      </c>
+      <c r="C7">
+        <v>2115</v>
+      </c>
       <c r="D7">
         <v>1330</v>
       </c>
@@ -1084,10 +1356,16 @@
         <v>1062</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:8">
       <c r="A8" s="1">
         <v>7</v>
       </c>
+      <c r="B8">
+        <v>5633</v>
+      </c>
+      <c r="C8">
+        <v>2303</v>
+      </c>
       <c r="D8">
         <v>1500</v>
       </c>
@@ -1098,10 +1376,16 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:8">
       <c r="A9" s="1">
         <v>8</v>
       </c>
+      <c r="B9">
+        <v>4176</v>
+      </c>
+      <c r="C9">
+        <v>1464</v>
+      </c>
       <c r="D9">
         <v>1074</v>
       </c>
@@ -1112,10 +1396,16 @@
         <v>885</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:8">
       <c r="A10" s="1">
         <v>9</v>
       </c>
+      <c r="B10">
+        <v>4295</v>
+      </c>
+      <c r="C10">
+        <v>1669</v>
+      </c>
       <c r="D10">
         <v>1231</v>
       </c>
@@ -1126,10 +1416,16 @@
         <v>861</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:8">
       <c r="A11" s="1">
         <v>10</v>
       </c>
+      <c r="B11">
+        <v>4866</v>
+      </c>
+      <c r="C11">
+        <v>1758</v>
+      </c>
       <c r="D11">
         <v>1072</v>
       </c>
@@ -1140,7 +1436,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:8">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1163,10 +1459,16 @@
         <v>151</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:8">
       <c r="A13" s="1">
         <v>12</v>
       </c>
+      <c r="B13">
+        <v>3965</v>
+      </c>
+      <c r="C13">
+        <v>1896</v>
+      </c>
       <c r="D13">
         <v>1771</v>
       </c>
@@ -1177,10 +1479,16 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:8">
       <c r="A14" s="1">
         <v>13</v>
       </c>
+      <c r="B14">
+        <v>5591</v>
+      </c>
+      <c r="C14">
+        <v>1979</v>
+      </c>
       <c r="D14">
         <v>1248</v>
       </c>
@@ -1191,10 +1499,16 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:8">
       <c r="A15" s="1">
         <v>14</v>
       </c>
+      <c r="B15">
+        <v>3728</v>
+      </c>
+      <c r="C15">
+        <v>1460</v>
+      </c>
       <c r="D15">
         <v>1039</v>
       </c>
@@ -1205,9 +1519,15 @@
         <v>752</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:8">
       <c r="A16" s="1">
         <v>15</v>
+      </c>
+      <c r="B16">
+        <v>5011</v>
+      </c>
+      <c r="C16">
+        <v>2579</v>
       </c>
       <c r="D16">
         <v>1097</v>
@@ -1223,6 +1543,12 @@
       <c r="A17" s="1">
         <v>16</v>
       </c>
+      <c r="B17">
+        <v>5266</v>
+      </c>
+      <c r="C17">
+        <v>1951</v>
+      </c>
       <c r="D17">
         <v>1296</v>
       </c>
@@ -1237,6 +1563,12 @@
       <c r="A18" s="1">
         <v>17</v>
       </c>
+      <c r="B18">
+        <v>5139</v>
+      </c>
+      <c r="C18">
+        <v>1712</v>
+      </c>
       <c r="D18">
         <v>1129</v>
       </c>
@@ -1251,6 +1583,12 @@
       <c r="A19" s="1">
         <v>18</v>
       </c>
+      <c r="B19">
+        <v>1184</v>
+      </c>
+      <c r="C19">
+        <v>581</v>
+      </c>
       <c r="D19">
         <v>548</v>
       </c>
@@ -1265,6 +1603,12 @@
       <c r="A20" s="1">
         <v>19</v>
       </c>
+      <c r="B20">
+        <v>4940</v>
+      </c>
+      <c r="C20">
+        <v>1982</v>
+      </c>
       <c r="D20">
         <v>979</v>
       </c>
@@ -1279,6 +1623,12 @@
       <c r="A21" s="1">
         <v>20</v>
       </c>
+      <c r="B21">
+        <v>7555</v>
+      </c>
+      <c r="C21">
+        <v>2405</v>
+      </c>
       <c r="D21">
         <v>1943</v>
       </c>
@@ -1292,6 +1642,12 @@
     <row r="22" spans="1:6">
       <c r="A22" s="1">
         <v>21</v>
+      </c>
+      <c r="B22">
+        <v>5358</v>
+      </c>
+      <c r="C22">
+        <v>1935</v>
       </c>
       <c r="D22">
         <v>1118</v>

</xml_diff>

<commit_message>
Actual version of diagrams.
</commit_message>
<xml_diff>
--- a/TimeTabling/doc/Solutions_Quality_Diagrams.xlsx
+++ b/TimeTabling/doc/Solutions_Quality_Diagrams.xlsx
@@ -11,9 +11,6 @@
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
@@ -111,10 +108,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>(Tabelle1!$B$1,Tabelle1!$C$1,Tabelle1!$F$1,Tabelle1!$G$1)</c:f>
+              <c:f>(Tabelle1!$B$1,Tabelle1!$C$1,Tabelle1!$F$1,Tabelle1!$G$1,Tabelle1!$I$1)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -126,16 +123,19 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Tabelle1!$B$2,Tabelle1!$C$2,Tabelle1!$F$2,Tabelle1!$G$2)</c:f>
+              <c:f>(Tabelle1!$B$2,Tabelle1!$C$2,Tabelle1!$F$2,Tabelle1!$G$2,Tabelle1!$I$2)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>1052</c:v>
                 </c:pt>
@@ -147,6 +147,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -160,10 +163,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>(Tabelle1!$B$1,Tabelle1!$C$1,Tabelle1!$F$1,Tabelle1!$G$1)</c:f>
+              <c:f>(Tabelle1!$B$1,Tabelle1!$C$1,Tabelle1!$F$1,Tabelle1!$G$1,Tabelle1!$I$1)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -175,6 +178,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -202,11 +208,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="74339072"/>
-        <c:axId val="74341376"/>
+        <c:axId val="57705600"/>
+        <c:axId val="57707904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="74339072"/>
+        <c:axId val="57705600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -232,14 +238,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74341376"/>
+        <c:crossAx val="57707904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="74341376"/>
+        <c:axId val="57707904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -265,7 +271,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74339072"/>
+        <c:crossAx val="57705600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -278,7 +284,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.70000000000000018" r="0.70000000000000018" t="0.78740157499999996" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000029" r="0.70000000000000029" t="0.78740157499999996" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -300,7 +306,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="de-DE"/>
-              <a:t>Instance11</a:t>
+              <a:t>Instance 11, 18</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -319,7 +325,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>(Tabelle1!$B$1:$C$1,Tabelle1!$F$1:$G$1)</c:f>
+              <c:f>(Tabelle1!$B$1,Tabelle1!$C$1,Tabelle1!$F$1,Tabelle1!$G$1)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -360,13 +366,61 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:hiLowLines/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Instance18</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>(Tabelle1!$B$1,Tabelle1!$C$1,Tabelle1!$F$1,Tabelle1!$G$1)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Tabelle1!$B$19,Tabelle1!$C$19,Tabelle1!$F$19,Tabelle1!$G$19)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1184</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>581</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>464</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>306</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
         <c:marker val="1"/>
-        <c:axId val="74362240"/>
-        <c:axId val="72947200"/>
+        <c:axId val="57729024"/>
+        <c:axId val="57730944"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="74362240"/>
+        <c:axId val="57729024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -392,14 +446,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72947200"/>
+        <c:crossAx val="57730944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72947200"/>
+        <c:axId val="57730944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -425,7 +479,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74362240"/>
+        <c:crossAx val="57729024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -438,7 +492,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7000000000000004" r="0.7000000000000004" t="0.78740157499999996" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000051" r="0.70000000000000051" t="0.78740157499999996" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -520,13 +574,61 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:hiLowLines/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Instance20</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>(Tabelle1!$B$1,Tabelle1!$C$1,Tabelle1!$F$1,Tabelle1!$G$1)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Tabelle1!$B$21,Tabelle1!$C$21,Tabelle1!$F$21,Tabelle1!$G$21)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>7555</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2405</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1521</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1050</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
         <c:marker val="1"/>
-        <c:axId val="73000832"/>
-        <c:axId val="73003008"/>
+        <c:axId val="58353920"/>
+        <c:axId val="58368384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="73000832"/>
+        <c:axId val="58353920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -552,14 +654,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73003008"/>
+        <c:crossAx val="58368384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="73003008"/>
+        <c:axId val="58368384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -585,7 +687,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73000832"/>
+        <c:crossAx val="58353920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -620,7 +722,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="de-DE"/>
-              <a:t>Instance03</a:t>
+              <a:t>Instance 03, 04</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -680,13 +782,61 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:hiLowLines/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Instance4</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>(Tabelle1!$B$1,Tabelle1!$C$1,Tabelle1!$F$1,Tabelle1!$G$1)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Tabelle1!$B$5,Tabelle1!$C$5,Tabelle1!$F$5,Tabelle1!$G$5)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4434</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1693</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>973</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>575</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
         <c:marker val="1"/>
-        <c:axId val="67409408"/>
-        <c:axId val="67411328"/>
+        <c:axId val="58790656"/>
+        <c:axId val="58792576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="67409408"/>
+        <c:axId val="58790656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -712,14 +862,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67411328"/>
+        <c:crossAx val="58792576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="67411328"/>
+        <c:axId val="58792576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -745,7 +895,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67409408"/>
+        <c:crossAx val="58790656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -799,15 +949,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>89</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -887,19 +1037,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Tabelle1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1187,10 +1324,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1198,7 +1335,7 @@
     <col min="1" max="1" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1">
+    <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1223,8 +1360,11 @@
       <c r="H1" s="1">
         <v>20000</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="1">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1249,8 +1389,11 @@
       <c r="H2">
         <v>138</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1273,7 +1416,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1296,7 +1439,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1315,8 +1458,11 @@
       <c r="F5">
         <v>973</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="G5">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1336,7 +1482,7 @@
         <v>2104</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1356,7 +1502,7 @@
         <v>1062</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1376,7 +1522,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:9">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1395,8 +1541,11 @@
       <c r="F9">
         <v>885</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="G9">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1416,7 +1565,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1436,7 +1585,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1459,7 +1608,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:9">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1479,7 +1628,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1499,7 +1648,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:9">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1519,7 +1668,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1539,7 +1688,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:7">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1559,7 +1708,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:7">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1579,7 +1728,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:7">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1598,8 +1747,11 @@
       <c r="F19">
         <v>464</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="G19">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1619,7 +1771,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:7">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1638,8 +1790,11 @@
       <c r="F21">
         <v>1521</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="G21">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="1">
         <v>21</v>
       </c>

</xml_diff>